<commit_message>
código de automacao de envio de mensagens por whatsApp
</commit_message>
<xml_diff>
--- a/enviados.xlsx
+++ b/enviados.xlsx
@@ -1,92 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REPOS\Automacao_NodeJs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ECA195-0649-438C-91E8-94111A2B8E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Enviados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
-  <si>
-    <t>beneficiario</t>
-  </si>
-  <si>
-    <t>celular</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>ANDRE FRISENE</t>
-  </si>
-  <si>
-    <t>5511994518634</t>
-  </si>
-  <si>
-    <t>enviado</t>
-  </si>
-  <si>
-    <t>2025-11-20T12:10:03.720Z</t>
-  </si>
-  <si>
-    <t>MARCELO MARTINHO</t>
-  </si>
-  <si>
-    <t>5511974992229</t>
-  </si>
-  <si>
-    <t>2025-11-20T12:10:05.674Z</t>
-  </si>
-  <si>
-    <t>LETICIA COSTA</t>
-  </si>
-  <si>
-    <t>5511913151311</t>
-  </si>
-  <si>
-    <t>2025-11-20T12:10:07.584Z</t>
-  </si>
-  <si>
-    <t>CAMILA MENESES</t>
-  </si>
-  <si>
-    <t>5513997261560</t>
-  </si>
-  <si>
-    <t>2025-11-20T12:10:10.638Z</t>
-  </si>
-  <si>
-    <t>FREITAS</t>
-  </si>
-  <si>
-    <t>5511996800701</t>
-  </si>
-  <si>
-    <t>2025-11-20T12:10:13.768Z</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -455,109 +396,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <sheetData/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D6" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>